<commit_message>
Armour finished + resiatnces etc. added
</commit_message>
<xml_diff>
--- a/CoreRulebook/Data/Items/tools.xlsx
+++ b/CoreRulebook/Data/Items/tools.xlsx
@@ -8,15 +8,23 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\HPRPG\CoreRulebook\Data\Items\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B53FCCC-3FD1-4742-999D-6660C20D6CBE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41284DFA-7DAE-4F0C-A5F1-8A776CF8895E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-90" windowWidth="29040" windowHeight="16440" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0" iterateDelta="1E-4"/>
+  <calcPr calcId="191029" iterateDelta="1E-4"/>
   <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="CalcA1"/>
     </ext>
@@ -129,9 +137,6 @@
     <t xml:space="preserve">A requirement for long-distance navigation. Allows you to chart a course for a on-foot travel, broomstick flight, ship\apos{}s course for journeys greater than 5 hour. Proficiency in these tools allows you to add 1 hour for every point of your Expertise bonus. </t>
   </si>
   <si>
-    <t xml:space="preserve">A set of tools for performing minor repairs to armour and clothing. Proficiency allows you to halve the time required to repair a set to full strength. </t>
-  </si>
-  <si>
     <t xml:space="preserve">Merely possessing a musical instrument allows you to make crude noises, but you require proficiency to truly play an instrument, and you may add your Expertise bonus to all checks relating to the instrument. Each subsequent instrument requires a new proficiency. </t>
   </si>
   <si>
@@ -139,6 +144,9 @@
   </si>
   <si>
     <t xml:space="preserve">A set of tools used to determine the authenticity and nature of mundane and magical objects, a Jeweller\apos{}s set bears a visual similarity to the muggle tools from which they get their name – an eyeglass and some simple alchemical equipment. Proficiency allows you to add your Expertise bonus to all checks used to determine the authenticity of an item. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">A set of tools for performing minor repairs to armour and clothing. Proficiency allows you to halve the time required to repair a set to full strength, and allows you to repair {\\it Destroyed} armour. </t>
   </si>
 </sst>
 </file>
@@ -494,8 +502,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -683,7 +691,7 @@
         <v>15</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="51" x14ac:dyDescent="0.2">
@@ -697,7 +705,7 @@
         <v>50</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="38.25" x14ac:dyDescent="0.2">
@@ -711,7 +719,7 @@
         <v>25</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="76.5" x14ac:dyDescent="0.2">
@@ -725,7 +733,7 @@
         <v>35</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>